<commit_message>
20200303 Update for examnple excel
</commit_message>
<xml_diff>
--- a/pattern_example.xlsx
+++ b/pattern_example.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5164CA09-4449-C845-BB56-1055E0D1BCB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16650" windowHeight="3300"/>
+    <workbookView xWindow="4340" yWindow="1340" windowWidth="16660" windowHeight="15060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PORT" sheetId="2" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>DISB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,10 +108,6 @@
   </si>
   <si>
     <t>SPI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">read </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -225,8 +222,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,28 +541,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" customWidth="1"/>
+    <col min="2" max="2" width="22.796875" customWidth="1"/>
+    <col min="3" max="3" width="32.59765625" customWidth="1"/>
+    <col min="4" max="4" width="16.3984375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="8" max="9" width="12.19921875" customWidth="1"/>
+    <col min="10" max="10" width="12.796875" customWidth="1"/>
+    <col min="11" max="11" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -582,27 +578,27 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
         <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -614,25 +610,25 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>46</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>47</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>48</v>
       </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -640,9 +636,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -653,22 +649,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.796875" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -682,25 +678,25 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -715,7 +711,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -730,69 +726,69 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5">
       <c r="E9" s="1"/>
     </row>
   </sheetData>

</xml_diff>